<commit_message>
Framework Setup - App elements, Steps and Tests
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Training\Mar_2025_930PM\AutomationTraining\AutomationMavenProject\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Training\Mar_2025_930PM\AutomationTraining\OrangeHRMTestNGFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B0CD5E-3C75-4DB0-82D1-78ADD3A979AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A335DA8B-F7FC-458D-B96A-1BA2874F5866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33480" yWindow="3090" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="verifyLoginPageLogoAndHeader" sheetId="3" r:id="rId1"/>
+    <sheet name="verifyLoginWithValidCredentials" sheetId="4" r:id="rId2"/>
+    <sheet name="verifyInvalidLogin" sheetId="7" r:id="rId3"/>
+    <sheet name="VerifyProfileImageInHomePage" sheetId="5" r:id="rId4"/>
+    <sheet name="VerifyHomePageMenus" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +29,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+  <si>
+    <t>LoginHeader</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
   <si>
     <t>Username</t>
   </si>
@@ -34,34 +43,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Role</t>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
   <si>
     <t>Bharath</t>
   </si>
   <si>
-    <t>Bharath123</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Bala</t>
-  </si>
-  <si>
-    <t>Bala123</t>
-  </si>
-  <si>
-    <t>Meghana</t>
-  </si>
-  <si>
-    <t>Mega123</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Employee</t>
+    <t>bharath123</t>
   </si>
 </sst>
 </file>
@@ -387,62 +378,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4ECE66A-8654-47FB-B225-99390EAD3D2D}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFD94C8-0339-4A8B-9759-038D879CE161}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -450,14 +441,99 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084FF9AB-30F3-4CC1-84E1-C3DD0B4BE6A2}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE8A700-757B-4515-A30F-16CF0C6B7D40}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4228218C-2E7B-47DA-B4E2-3369CEB4B140}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24483F-75C1-4590-A9AA-836D6C169F4E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>